<commit_message>
Ajustes en el formato para registrados por empresa
</commit_message>
<xml_diff>
--- a/docs/formatos/participantesEmpresa.xlsx
+++ b/docs/formatos/participantesEmpresa.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,26 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Código</t>
   </si>
   <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Fecha de Registro</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
     <t>País</t>
   </si>
   <si>
@@ -57,14 +42,35 @@
     <t>Campo4</t>
   </si>
   <si>
-    <t>Fecha de Nacimiento</t>
+    <t>Usuario / Login</t>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Fecha de registro</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Activo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,19 +92,25 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,11 +144,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -147,9 +172,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,100 +468,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" customWidth="1"/>
-    <col min="7" max="7" width="54" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="40" customWidth="1"/>
-    <col min="10" max="10" width="35.5703125" customWidth="1"/>
-    <col min="11" max="11" width="37.85546875" customWidth="1"/>
-    <col min="12" max="12" width="38.140625" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>11</v>
+      <c r="O4" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -538,13 +589,13 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="4"/>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>